<commit_message>
2.0 Baseline after Incr-1; after Teraza left FYP
2.0	5/9/2018	Balasubramanian Narasimhan	Baseline version after Incr-1
</commit_message>
<xml_diff>
--- a/MGMT/PLAN/PP/WORK IN PROGRESS/RAM_MRP.xlsx
+++ b/MGMT/PLAN/PP/WORK IN PROGRESS/RAM_MRP.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="175">
   <si>
     <t>Risk Item</t>
   </si>
@@ -511,15 +511,9 @@
     <t xml:space="preserve">The technical landscape is new to the entire team, and requires each one of us to undertstand the teachnicalities to contribute effectively to the project </t>
   </si>
   <si>
-    <t>Requesting the client to provide us with actual/physical devices so as to get a practical understanding while mapping the functionalities and planning for activities beyond coding</t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
-    <t>Baselining URS</t>
-  </si>
-  <si>
     <t>Development phase</t>
   </si>
   <si>
@@ -538,9 +532,6 @@
     <t>Bala took over the URS preparation and reviewed it within the team, before being circulated to the client</t>
   </si>
   <si>
-    <t>There could be unknown issues arising while capturing data from actual device</t>
-  </si>
-  <si>
     <t>In the proto type, the windows machine is as acting as the device and sending signals.</t>
   </si>
   <si>
@@ -556,10 +547,34 @@
     <t>In the proto type, the windows machine is as acting as the device and sending limited set of data signals.</t>
   </si>
   <si>
-    <t>Request SERIS to share the detailed requirements along with data samples.  Besides the no of devices and expected throughput from the RAM application</t>
-  </si>
-  <si>
     <t>Request SERIS to provide us data samples.  Request SERIS to help cnfigure a device to send data to RAM proto type</t>
+  </si>
+  <si>
+    <t>Baselining URS; 5-Sep the URS was baselined</t>
+  </si>
+  <si>
+    <t>Request SERIS to share the detailed requirements along with data samples.  Besides the no of devices and expected throughput from the RAM application; SERIS requested us to perform simulation testing</t>
+  </si>
+  <si>
+    <t>Requesting the client to provide us with actual/physical devices so as to get a practical understanding while mapping the functionalities and planning for activities beyond coding; The URS was bsaedline on 5-Sep, except for a few components to be addressed in Iteration-2</t>
+  </si>
+  <si>
+    <t>Risk realized in Oct and accepted by the team; The team decided to split the workload of the team member who left</t>
+  </si>
+  <si>
+    <t>Client has asked us to look in to the possibility of taking in JSON format data</t>
+  </si>
+  <si>
+    <t>if there is a change in the source data feed, it will have a greater end-to-end to the project.</t>
+  </si>
+  <si>
+    <t>Stakeholder engagement, Oct-2018</t>
+  </si>
+  <si>
+    <t>However this means there is a considerable re-work from URS all the way into testing which has already been completed for and until increment-1.   The team agreed to accept the risk in the best interest of meeting client requirements as they fit is best for their use case.</t>
+  </si>
+  <si>
+    <t>There could be unknown issues arising while capturing data from actual device/station</t>
   </si>
 </sst>
 </file>
@@ -722,7 +737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1141,41 +1156,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1183,7 +1163,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1283,27 +1263,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1319,6 +1278,27 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1328,7 +1308,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1340,8 +1319,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1360,24 +1337,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1968,11 +1927,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG16"/>
+  <dimension ref="A1:DG17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1991,39 +1950,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:111" s="42" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="J1" s="49" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:111" s="42" customFormat="1" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57">
+      <c r="A2" s="50">
         <v>1</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -2048,14 +2007,14 @@
         <v>113</v>
       </c>
       <c r="I2" s="43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J2" s="44" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:111" s="42" customFormat="1" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57">
+      <c r="A3" s="50">
         <v>2</v>
       </c>
       <c r="B3" s="45" t="s">
@@ -2079,13 +2038,15 @@
       <c r="H3" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="45"/>
+      <c r="I3" s="45" t="s">
+        <v>114</v>
+      </c>
       <c r="J3" s="46" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:111" s="42" customFormat="1" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57">
+      <c r="A4" s="50">
         <v>3</v>
       </c>
       <c r="B4" s="43" t="s">
@@ -2117,17 +2078,17 @@
       </c>
     </row>
     <row r="5" spans="1:111" s="42" customFormat="1" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57">
+      <c r="A5" s="50">
         <v>4</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" s="45" t="s">
         <v>110</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>111</v>
@@ -2136,30 +2097,30 @@
         <v>70</v>
       </c>
       <c r="G5" s="45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>114</v>
       </c>
       <c r="J5" s="46" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:111" s="42" customFormat="1" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57">
+      <c r="A6" s="50">
         <v>5</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C6" s="43" t="s">
         <v>121</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E6" s="43" t="s">
         <v>118</v>
@@ -2168,18 +2129,20 @@
         <v>64</v>
       </c>
       <c r="G6" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H6" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="43"/>
+      <c r="I6" s="43" t="s">
+        <v>114</v>
+      </c>
       <c r="J6" s="44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:111" s="15" customFormat="1" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="57">
+      <c r="A7" s="50">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
@@ -2312,7 +2275,7 @@
       <c r="DG7" s="14"/>
     </row>
     <row r="8" spans="1:111" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57">
+      <c r="A8" s="50">
         <v>7</v>
       </c>
       <c r="B8" s="45" t="s">
@@ -2337,10 +2300,10 @@
         <v>113</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="J8" s="46" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
@@ -2445,17 +2408,17 @@
       <c r="DG8" s="16"/>
     </row>
     <row r="9" spans="1:111" s="42" customFormat="1" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57">
+      <c r="A9" s="50">
         <v>8</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C9" s="43" t="s">
         <v>121</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>118</v>
@@ -2464,28 +2427,30 @@
         <v>64</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H9" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="I9" s="43"/>
+      <c r="I9" s="43" t="s">
+        <v>153</v>
+      </c>
       <c r="J9" s="44" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:111" s="42" customFormat="1" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57">
+      <c r="A10" s="50">
         <v>9</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C10" s="45" t="s">
         <v>110</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E10" s="45" t="s">
         <v>111</v>
@@ -2499,20 +2464,44 @@
       <c r="H10" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
-    </row>
-    <row r="11" spans="1:111" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="I10" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="J10" s="46" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:111" ht="79.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51">
+        <v>10</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="45" t="s">
+        <v>173</v>
+      </c>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
@@ -2615,8 +2604,10 @@
       <c r="DF11" s="16"/>
       <c r="DG11" s="16"/>
     </row>
-    <row r="12" spans="1:111" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
+    <row r="12" spans="1:111" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="50">
+        <v>11</v>
+      </c>
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -2728,17 +2719,19 @@
       <c r="DF12" s="16"/>
       <c r="DG12" s="16"/>
     </row>
-    <row r="13" spans="1:111" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="49"/>
+    <row r="13" spans="1:111" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="51">
+        <v>12</v>
+      </c>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
@@ -2841,17 +2834,19 @@
       <c r="DF13" s="16"/>
       <c r="DG13" s="16"/>
     </row>
-    <row r="14" spans="1:111" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="49"/>
+    <row r="14" spans="1:111" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="50">
+        <v>13</v>
+      </c>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="46"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
@@ -2954,17 +2949,19 @@
       <c r="DF14" s="16"/>
       <c r="DG14" s="16"/>
     </row>
-    <row r="15" spans="1:111" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
+    <row r="15" spans="1:111" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="51">
+        <v>14</v>
+      </c>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -3067,17 +3064,19 @@
       <c r="DF15" s="16"/>
       <c r="DG15" s="16"/>
     </row>
-    <row r="16" spans="1:111" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
+    <row r="16" spans="1:111" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="50">
+        <v>15</v>
+      </c>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="46"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -3180,6 +3179,18 @@
       <c r="DF16" s="16"/>
       <c r="DG16" s="16"/>
     </row>
+    <row r="17" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3206,15 +3217,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="72"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="19"/>
@@ -3224,42 +3235,42 @@
       <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
     </row>
     <row r="3" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="64"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="69"/>
     </row>
     <row r="4" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
@@ -3380,30 +3391,30 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
-      <c r="X10" s="69"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="53"/>
+      <c r="Q10" s="53"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53"/>
+      <c r="T10" s="53"/>
+      <c r="U10" s="53"/>
+      <c r="V10" s="53"/>
+      <c r="W10" s="53"/>
+      <c r="X10" s="53"/>
     </row>
     <row r="11" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
@@ -3412,13 +3423,13 @@
       <c r="B11" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="72"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:24" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -3427,13 +3438,13 @@
       <c r="B12" s="40">
         <v>5</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:24" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
@@ -3442,13 +3453,13 @@
       <c r="B13" s="40">
         <v>4</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="78"/>
     </row>
     <row r="14" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
@@ -3457,13 +3468,13 @@
       <c r="B14" s="40">
         <v>3</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="75"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="15" spans="1:24" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
@@ -3472,13 +3483,13 @@
       <c r="B15" s="40">
         <v>2</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="78"/>
     </row>
     <row r="16" spans="1:24" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
@@ -3487,1165 +3498,1141 @@
       <c r="B16" s="41">
         <v>1</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
     </row>
     <row r="17" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="69"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="69"/>
-      <c r="W17" s="69"/>
-      <c r="X17" s="69"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
     </row>
     <row r="18" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="62" t="s">
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="85"/>
+      <c r="G18" s="64"/>
     </row>
     <row r="19" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="79" t="s">
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="83"/>
+      <c r="G19" s="61"/>
     </row>
     <row r="20" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="79" t="s">
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="83"/>
+      <c r="G20" s="61"/>
     </row>
     <row r="21" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="79" t="s">
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="83"/>
+      <c r="G21" s="61"/>
     </row>
     <row r="22" spans="1:24" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="81" t="s">
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="G22" s="84"/>
+      <c r="G22" s="62"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="68"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="69"/>
-      <c r="O23" s="69"/>
-      <c r="P23" s="69"/>
-      <c r="Q23" s="69"/>
-      <c r="R23" s="69"/>
-      <c r="S23" s="69"/>
-      <c r="T23" s="69"/>
-      <c r="U23" s="69"/>
-      <c r="V23" s="69"/>
-      <c r="W23" s="69"/>
-      <c r="X23" s="69"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
+      <c r="T23" s="53"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="68"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-      <c r="O24" s="69"/>
-      <c r="P24" s="69"/>
-      <c r="Q24" s="69"/>
-      <c r="R24" s="69"/>
-      <c r="S24" s="69"/>
-      <c r="T24" s="69"/>
-      <c r="U24" s="69"/>
-      <c r="V24" s="69"/>
-      <c r="W24" s="69"/>
-      <c r="X24" s="69"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
+      <c r="T24" s="53"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="68"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
-      <c r="Q25" s="69"/>
-      <c r="R25" s="69"/>
-      <c r="S25" s="69"/>
-      <c r="T25" s="69"/>
-      <c r="U25" s="69"/>
-      <c r="V25" s="69"/>
-      <c r="W25" s="69"/>
-      <c r="X25" s="69"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="53"/>
+      <c r="T25" s="53"/>
+      <c r="U25" s="53"/>
+      <c r="V25" s="53"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="53"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="68"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="69"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="69"/>
-      <c r="Q26" s="69"/>
-      <c r="R26" s="69"/>
-      <c r="S26" s="69"/>
-      <c r="T26" s="69"/>
-      <c r="U26" s="69"/>
-      <c r="V26" s="69"/>
-      <c r="W26" s="69"/>
-      <c r="X26" s="69"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="53"/>
+      <c r="T26" s="53"/>
+      <c r="U26" s="53"/>
+      <c r="V26" s="53"/>
+      <c r="W26" s="53"/>
+      <c r="X26" s="53"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
-      <c r="M27" s="69"/>
-      <c r="N27" s="69"/>
-      <c r="O27" s="69"/>
-      <c r="P27" s="69"/>
-      <c r="Q27" s="69"/>
-      <c r="R27" s="69"/>
-      <c r="S27" s="69"/>
-      <c r="T27" s="69"/>
-      <c r="U27" s="69"/>
-      <c r="V27" s="69"/>
-      <c r="W27" s="69"/>
-      <c r="X27" s="69"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53"/>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="53"/>
+      <c r="X27" s="53"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="68"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-      <c r="Q28" s="69"/>
-      <c r="R28" s="69"/>
-      <c r="S28" s="69"/>
-      <c r="T28" s="69"/>
-      <c r="U28" s="69"/>
-      <c r="V28" s="69"/>
-      <c r="W28" s="69"/>
-      <c r="X28" s="69"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="53"/>
+      <c r="T28" s="53"/>
+      <c r="U28" s="53"/>
+      <c r="V28" s="53"/>
+      <c r="W28" s="53"/>
+      <c r="X28" s="53"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="69"/>
-      <c r="R29" s="69"/>
-      <c r="S29" s="69"/>
-      <c r="T29" s="69"/>
-      <c r="U29" s="69"/>
-      <c r="V29" s="69"/>
-      <c r="W29" s="69"/>
-      <c r="X29" s="69"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="53"/>
+      <c r="W29" s="53"/>
+      <c r="X29" s="53"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="68"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="69"/>
-      <c r="R30" s="69"/>
-      <c r="S30" s="69"/>
-      <c r="T30" s="69"/>
-      <c r="U30" s="69"/>
-      <c r="V30" s="69"/>
-      <c r="W30" s="69"/>
-      <c r="X30" s="69"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="53"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="53"/>
+      <c r="X30" s="53"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="69"/>
-      <c r="R31" s="69"/>
-      <c r="S31" s="69"/>
-      <c r="T31" s="69"/>
-      <c r="U31" s="69"/>
-      <c r="V31" s="69"/>
-      <c r="W31" s="69"/>
-      <c r="X31" s="69"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="53"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="53"/>
+      <c r="T31" s="53"/>
+      <c r="U31" s="53"/>
+      <c r="V31" s="53"/>
+      <c r="W31" s="53"/>
+      <c r="X31" s="53"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="68"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="69"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="69"/>
-      <c r="R32" s="69"/>
-      <c r="S32" s="69"/>
-      <c r="T32" s="69"/>
-      <c r="U32" s="69"/>
-      <c r="V32" s="69"/>
-      <c r="W32" s="69"/>
-      <c r="X32" s="69"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
+      <c r="N32" s="53"/>
+      <c r="O32" s="53"/>
+      <c r="P32" s="53"/>
+      <c r="Q32" s="53"/>
+      <c r="R32" s="53"/>
+      <c r="S32" s="53"/>
+      <c r="T32" s="53"/>
+      <c r="U32" s="53"/>
+      <c r="V32" s="53"/>
+      <c r="W32" s="53"/>
+      <c r="X32" s="53"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="68"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="69"/>
-      <c r="R33" s="69"/>
-      <c r="S33" s="69"/>
-      <c r="T33" s="69"/>
-      <c r="U33" s="69"/>
-      <c r="V33" s="69"/>
-      <c r="W33" s="69"/>
-      <c r="X33" s="69"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="53"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="53"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
+      <c r="T33" s="53"/>
+      <c r="U33" s="53"/>
+      <c r="V33" s="53"/>
+      <c r="W33" s="53"/>
+      <c r="X33" s="53"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="68"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="69"/>
-      <c r="M34" s="69"/>
-      <c r="N34" s="69"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="69"/>
-      <c r="R34" s="69"/>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="69"/>
-      <c r="W34" s="69"/>
-      <c r="X34" s="69"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="53"/>
+      <c r="O34" s="53"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="53"/>
+      <c r="R34" s="53"/>
+      <c r="S34" s="53"/>
+      <c r="T34" s="53"/>
+      <c r="U34" s="53"/>
+      <c r="V34" s="53"/>
+      <c r="W34" s="53"/>
+      <c r="X34" s="53"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="69"/>
-      <c r="N35" s="69"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="69"/>
-      <c r="R35" s="69"/>
-      <c r="S35" s="69"/>
-      <c r="T35" s="69"/>
-      <c r="U35" s="69"/>
-      <c r="V35" s="69"/>
-      <c r="W35" s="69"/>
-      <c r="X35" s="69"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="53"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="53"/>
+      <c r="T35" s="53"/>
+      <c r="U35" s="53"/>
+      <c r="V35" s="53"/>
+      <c r="W35" s="53"/>
+      <c r="X35" s="53"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="68"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="69"/>
-      <c r="L36" s="69"/>
-      <c r="M36" s="69"/>
-      <c r="N36" s="69"/>
-      <c r="O36" s="69"/>
-      <c r="P36" s="69"/>
-      <c r="Q36" s="69"/>
-      <c r="R36" s="69"/>
-      <c r="S36" s="69"/>
-      <c r="T36" s="69"/>
-      <c r="U36" s="69"/>
-      <c r="V36" s="69"/>
-      <c r="W36" s="69"/>
-      <c r="X36" s="69"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="53"/>
+      <c r="O36" s="53"/>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="53"/>
+      <c r="T36" s="53"/>
+      <c r="U36" s="53"/>
+      <c r="V36" s="53"/>
+      <c r="W36" s="53"/>
+      <c r="X36" s="53"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="68"/>
-      <c r="B37" s="69"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="69"/>
-      <c r="N37" s="69"/>
-      <c r="O37" s="69"/>
-      <c r="P37" s="69"/>
-      <c r="Q37" s="69"/>
-      <c r="R37" s="69"/>
-      <c r="S37" s="69"/>
-      <c r="T37" s="69"/>
-      <c r="U37" s="69"/>
-      <c r="V37" s="69"/>
-      <c r="W37" s="69"/>
-      <c r="X37" s="69"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="53"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="53"/>
+      <c r="Q37" s="53"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="53"/>
+      <c r="T37" s="53"/>
+      <c r="U37" s="53"/>
+      <c r="V37" s="53"/>
+      <c r="W37" s="53"/>
+      <c r="X37" s="53"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A38" s="68"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="69"/>
-      <c r="K38" s="69"/>
-      <c r="L38" s="69"/>
-      <c r="M38" s="69"/>
-      <c r="N38" s="69"/>
-      <c r="O38" s="69"/>
-      <c r="P38" s="69"/>
-      <c r="Q38" s="69"/>
-      <c r="R38" s="69"/>
-      <c r="S38" s="69"/>
-      <c r="T38" s="69"/>
-      <c r="U38" s="69"/>
-      <c r="V38" s="69"/>
-      <c r="W38" s="69"/>
-      <c r="X38" s="69"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="53"/>
+      <c r="O38" s="53"/>
+      <c r="P38" s="53"/>
+      <c r="Q38" s="53"/>
+      <c r="R38" s="53"/>
+      <c r="S38" s="53"/>
+      <c r="T38" s="53"/>
+      <c r="U38" s="53"/>
+      <c r="V38" s="53"/>
+      <c r="W38" s="53"/>
+      <c r="X38" s="53"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A39" s="68"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
-      <c r="J39" s="69"/>
-      <c r="K39" s="69"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="69"/>
-      <c r="N39" s="69"/>
-      <c r="O39" s="69"/>
-      <c r="P39" s="69"/>
-      <c r="Q39" s="69"/>
-      <c r="R39" s="69"/>
-      <c r="S39" s="69"/>
-      <c r="T39" s="69"/>
-      <c r="U39" s="69"/>
-      <c r="V39" s="69"/>
-      <c r="W39" s="69"/>
-      <c r="X39" s="69"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="53"/>
+      <c r="R39" s="53"/>
+      <c r="S39" s="53"/>
+      <c r="T39" s="53"/>
+      <c r="U39" s="53"/>
+      <c r="V39" s="53"/>
+      <c r="W39" s="53"/>
+      <c r="X39" s="53"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A40" s="68"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="69"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="69"/>
-      <c r="J40" s="69"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="69"/>
-      <c r="N40" s="69"/>
-      <c r="O40" s="69"/>
-      <c r="P40" s="69"/>
-      <c r="Q40" s="69"/>
-      <c r="R40" s="69"/>
-      <c r="S40" s="69"/>
-      <c r="T40" s="69"/>
-      <c r="U40" s="69"/>
-      <c r="V40" s="69"/>
-      <c r="W40" s="69"/>
-      <c r="X40" s="69"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="53"/>
+      <c r="T40" s="53"/>
+      <c r="U40" s="53"/>
+      <c r="V40" s="53"/>
+      <c r="W40" s="53"/>
+      <c r="X40" s="53"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A41" s="68"/>
-      <c r="B41" s="69"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="69"/>
-      <c r="J41" s="69"/>
-      <c r="K41" s="69"/>
-      <c r="L41" s="69"/>
-      <c r="M41" s="69"/>
-      <c r="N41" s="69"/>
-      <c r="O41" s="69"/>
-      <c r="P41" s="69"/>
-      <c r="Q41" s="69"/>
-      <c r="R41" s="69"/>
-      <c r="S41" s="69"/>
-      <c r="T41" s="69"/>
-      <c r="U41" s="69"/>
-      <c r="V41" s="69"/>
-      <c r="W41" s="69"/>
-      <c r="X41" s="69"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="53"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="68"/>
-      <c r="B42" s="69"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="69"/>
-      <c r="O42" s="69"/>
-      <c r="P42" s="69"/>
-      <c r="Q42" s="69"/>
-      <c r="R42" s="69"/>
-      <c r="S42" s="69"/>
-      <c r="T42" s="69"/>
-      <c r="U42" s="69"/>
-      <c r="V42" s="69"/>
-      <c r="W42" s="69"/>
-      <c r="X42" s="69"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="53"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A43" s="68"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="69"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="69"/>
-      <c r="J43" s="69"/>
-      <c r="K43" s="69"/>
-      <c r="L43" s="69"/>
-      <c r="M43" s="69"/>
-      <c r="N43" s="69"/>
-      <c r="O43" s="69"/>
-      <c r="P43" s="69"/>
-      <c r="Q43" s="69"/>
-      <c r="R43" s="69"/>
-      <c r="S43" s="69"/>
-      <c r="T43" s="69"/>
-      <c r="U43" s="69"/>
-      <c r="V43" s="69"/>
-      <c r="W43" s="69"/>
-      <c r="X43" s="69"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="53"/>
+      <c r="W43" s="53"/>
+      <c r="X43" s="53"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A44" s="68"/>
-      <c r="B44" s="69"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="69"/>
-      <c r="J44" s="69"/>
-      <c r="K44" s="69"/>
-      <c r="L44" s="69"/>
-      <c r="M44" s="69"/>
-      <c r="N44" s="69"/>
-      <c r="O44" s="69"/>
-      <c r="P44" s="69"/>
-      <c r="Q44" s="69"/>
-      <c r="R44" s="69"/>
-      <c r="S44" s="69"/>
-      <c r="T44" s="69"/>
-      <c r="U44" s="69"/>
-      <c r="V44" s="69"/>
-      <c r="W44" s="69"/>
-      <c r="X44" s="69"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="53"/>
+      <c r="R44" s="53"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="53"/>
+      <c r="W44" s="53"/>
+      <c r="X44" s="53"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A45" s="68"/>
-      <c r="B45" s="69"/>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="69"/>
-      <c r="J45" s="69"/>
-      <c r="K45" s="69"/>
-      <c r="L45" s="69"/>
-      <c r="M45" s="69"/>
-      <c r="N45" s="69"/>
-      <c r="O45" s="69"/>
-      <c r="P45" s="69"/>
-      <c r="Q45" s="69"/>
-      <c r="R45" s="69"/>
-      <c r="S45" s="69"/>
-      <c r="T45" s="69"/>
-      <c r="U45" s="69"/>
-      <c r="V45" s="69"/>
-      <c r="W45" s="69"/>
-      <c r="X45" s="69"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="53"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="53"/>
+      <c r="S45" s="53"/>
+      <c r="T45" s="53"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="53"/>
+      <c r="W45" s="53"/>
+      <c r="X45" s="53"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A46" s="68"/>
-      <c r="B46" s="69"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="69"/>
-      <c r="I46" s="69"/>
-      <c r="J46" s="69"/>
-      <c r="K46" s="69"/>
-      <c r="L46" s="69"/>
-      <c r="M46" s="69"/>
-      <c r="N46" s="69"/>
-      <c r="O46" s="69"/>
-      <c r="P46" s="69"/>
-      <c r="Q46" s="69"/>
-      <c r="R46" s="69"/>
-      <c r="S46" s="69"/>
-      <c r="T46" s="69"/>
-      <c r="U46" s="69"/>
-      <c r="V46" s="69"/>
-      <c r="W46" s="69"/>
-      <c r="X46" s="69"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="53"/>
+      <c r="M46" s="53"/>
+      <c r="N46" s="53"/>
+      <c r="O46" s="53"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="53"/>
+      <c r="R46" s="53"/>
+      <c r="S46" s="53"/>
+      <c r="T46" s="53"/>
+      <c r="U46" s="53"/>
+      <c r="V46" s="53"/>
+      <c r="W46" s="53"/>
+      <c r="X46" s="53"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A47" s="68"/>
-      <c r="B47" s="69"/>
-      <c r="C47" s="69"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="69"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="69"/>
-      <c r="I47" s="69"/>
-      <c r="J47" s="69"/>
-      <c r="K47" s="69"/>
-      <c r="L47" s="69"/>
-      <c r="M47" s="69"/>
-      <c r="N47" s="69"/>
-      <c r="O47" s="69"/>
-      <c r="P47" s="69"/>
-      <c r="Q47" s="69"/>
-      <c r="R47" s="69"/>
-      <c r="S47" s="69"/>
-      <c r="T47" s="69"/>
-      <c r="U47" s="69"/>
-      <c r="V47" s="69"/>
-      <c r="W47" s="69"/>
-      <c r="X47" s="69"/>
+      <c r="A47" s="52"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
+      <c r="L47" s="53"/>
+      <c r="M47" s="53"/>
+      <c r="N47" s="53"/>
+      <c r="O47" s="53"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="53"/>
+      <c r="S47" s="53"/>
+      <c r="T47" s="53"/>
+      <c r="U47" s="53"/>
+      <c r="V47" s="53"/>
+      <c r="W47" s="53"/>
+      <c r="X47" s="53"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A48" s="68"/>
-      <c r="B48" s="69"/>
-      <c r="C48" s="69"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="69"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="69"/>
-      <c r="J48" s="69"/>
-      <c r="K48" s="69"/>
-      <c r="L48" s="69"/>
-      <c r="M48" s="69"/>
-      <c r="N48" s="69"/>
-      <c r="O48" s="69"/>
-      <c r="P48" s="69"/>
-      <c r="Q48" s="69"/>
-      <c r="R48" s="69"/>
-      <c r="S48" s="69"/>
-      <c r="T48" s="69"/>
-      <c r="U48" s="69"/>
-      <c r="V48" s="69"/>
-      <c r="W48" s="69"/>
-      <c r="X48" s="69"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="53"/>
+      <c r="T48" s="53"/>
+      <c r="U48" s="53"/>
+      <c r="V48" s="53"/>
+      <c r="W48" s="53"/>
+      <c r="X48" s="53"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A49" s="68"/>
-      <c r="B49" s="69"/>
-      <c r="C49" s="69"/>
-      <c r="D49" s="69"/>
-      <c r="E49" s="69"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="69"/>
-      <c r="I49" s="69"/>
-      <c r="J49" s="69"/>
-      <c r="K49" s="69"/>
-      <c r="L49" s="69"/>
-      <c r="M49" s="69"/>
-      <c r="N49" s="69"/>
-      <c r="O49" s="69"/>
-      <c r="P49" s="69"/>
-      <c r="Q49" s="69"/>
-      <c r="R49" s="69"/>
-      <c r="S49" s="69"/>
-      <c r="T49" s="69"/>
-      <c r="U49" s="69"/>
-      <c r="V49" s="69"/>
-      <c r="W49" s="69"/>
-      <c r="X49" s="69"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="53"/>
+      <c r="L49" s="53"/>
+      <c r="M49" s="53"/>
+      <c r="N49" s="53"/>
+      <c r="O49" s="53"/>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="53"/>
+      <c r="R49" s="53"/>
+      <c r="S49" s="53"/>
+      <c r="T49" s="53"/>
+      <c r="U49" s="53"/>
+      <c r="V49" s="53"/>
+      <c r="W49" s="53"/>
+      <c r="X49" s="53"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A50" s="68"/>
-      <c r="B50" s="69"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="69"/>
-      <c r="K50" s="69"/>
-      <c r="L50" s="69"/>
-      <c r="M50" s="69"/>
-      <c r="N50" s="69"/>
-      <c r="O50" s="69"/>
-      <c r="P50" s="69"/>
-      <c r="Q50" s="69"/>
-      <c r="R50" s="69"/>
-      <c r="S50" s="69"/>
-      <c r="T50" s="69"/>
-      <c r="U50" s="69"/>
-      <c r="V50" s="69"/>
-      <c r="W50" s="69"/>
-      <c r="X50" s="69"/>
+      <c r="A50" s="52"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="53"/>
+      <c r="N50" s="53"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="53"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="53"/>
+      <c r="S50" s="53"/>
+      <c r="T50" s="53"/>
+      <c r="U50" s="53"/>
+      <c r="V50" s="53"/>
+      <c r="W50" s="53"/>
+      <c r="X50" s="53"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A51" s="68"/>
-      <c r="B51" s="69"/>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="69"/>
-      <c r="G51" s="69"/>
-      <c r="H51" s="69"/>
-      <c r="I51" s="69"/>
-      <c r="J51" s="69"/>
-      <c r="K51" s="69"/>
-      <c r="L51" s="69"/>
-      <c r="M51" s="69"/>
-      <c r="N51" s="69"/>
-      <c r="O51" s="69"/>
-      <c r="P51" s="69"/>
-      <c r="Q51" s="69"/>
-      <c r="R51" s="69"/>
-      <c r="S51" s="69"/>
-      <c r="T51" s="69"/>
-      <c r="U51" s="69"/>
-      <c r="V51" s="69"/>
-      <c r="W51" s="69"/>
-      <c r="X51" s="69"/>
+      <c r="A51" s="52"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="53"/>
+      <c r="L51" s="53"/>
+      <c r="M51" s="53"/>
+      <c r="N51" s="53"/>
+      <c r="O51" s="53"/>
+      <c r="P51" s="53"/>
+      <c r="Q51" s="53"/>
+      <c r="R51" s="53"/>
+      <c r="S51" s="53"/>
+      <c r="T51" s="53"/>
+      <c r="U51" s="53"/>
+      <c r="V51" s="53"/>
+      <c r="W51" s="53"/>
+      <c r="X51" s="53"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A52" s="68"/>
-      <c r="B52" s="69"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="69"/>
-      <c r="G52" s="69"/>
-      <c r="H52" s="69"/>
-      <c r="I52" s="69"/>
-      <c r="J52" s="69"/>
-      <c r="K52" s="69"/>
-      <c r="L52" s="69"/>
-      <c r="M52" s="69"/>
-      <c r="N52" s="69"/>
-      <c r="O52" s="69"/>
-      <c r="P52" s="69"/>
-      <c r="Q52" s="69"/>
-      <c r="R52" s="69"/>
-      <c r="S52" s="69"/>
-      <c r="T52" s="69"/>
-      <c r="U52" s="69"/>
-      <c r="V52" s="69"/>
-      <c r="W52" s="69"/>
-      <c r="X52" s="69"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="53"/>
+      <c r="L52" s="53"/>
+      <c r="M52" s="53"/>
+      <c r="N52" s="53"/>
+      <c r="O52" s="53"/>
+      <c r="P52" s="53"/>
+      <c r="Q52" s="53"/>
+      <c r="R52" s="53"/>
+      <c r="S52" s="53"/>
+      <c r="T52" s="53"/>
+      <c r="U52" s="53"/>
+      <c r="V52" s="53"/>
+      <c r="W52" s="53"/>
+      <c r="X52" s="53"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A53" s="68"/>
-      <c r="B53" s="69"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="69"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
-      <c r="G53" s="69"/>
-      <c r="H53" s="69"/>
-      <c r="I53" s="69"/>
-      <c r="J53" s="69"/>
-      <c r="K53" s="69"/>
-      <c r="L53" s="69"/>
-      <c r="M53" s="69"/>
-      <c r="N53" s="69"/>
-      <c r="O53" s="69"/>
-      <c r="P53" s="69"/>
-      <c r="Q53" s="69"/>
-      <c r="R53" s="69"/>
-      <c r="S53" s="69"/>
-      <c r="T53" s="69"/>
-      <c r="U53" s="69"/>
-      <c r="V53" s="69"/>
-      <c r="W53" s="69"/>
-      <c r="X53" s="69"/>
+      <c r="A53" s="52"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="53"/>
+      <c r="M53" s="53"/>
+      <c r="N53" s="53"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="53"/>
+      <c r="Q53" s="53"/>
+      <c r="R53" s="53"/>
+      <c r="S53" s="53"/>
+      <c r="T53" s="53"/>
+      <c r="U53" s="53"/>
+      <c r="V53" s="53"/>
+      <c r="W53" s="53"/>
+      <c r="X53" s="53"/>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A54" s="68"/>
-      <c r="B54" s="69"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="69"/>
-      <c r="E54" s="69"/>
-      <c r="F54" s="69"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="69"/>
-      <c r="I54" s="69"/>
-      <c r="J54" s="69"/>
-      <c r="K54" s="69"/>
-      <c r="L54" s="69"/>
-      <c r="M54" s="69"/>
-      <c r="N54" s="69"/>
-      <c r="O54" s="69"/>
-      <c r="P54" s="69"/>
-      <c r="Q54" s="69"/>
-      <c r="R54" s="69"/>
-      <c r="S54" s="69"/>
-      <c r="T54" s="69"/>
-      <c r="U54" s="69"/>
-      <c r="V54" s="69"/>
-      <c r="W54" s="69"/>
-      <c r="X54" s="69"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="53"/>
+      <c r="L54" s="53"/>
+      <c r="M54" s="53"/>
+      <c r="N54" s="53"/>
+      <c r="O54" s="53"/>
+      <c r="P54" s="53"/>
+      <c r="Q54" s="53"/>
+      <c r="R54" s="53"/>
+      <c r="S54" s="53"/>
+      <c r="T54" s="53"/>
+      <c r="U54" s="53"/>
+      <c r="V54" s="53"/>
+      <c r="W54" s="53"/>
+      <c r="X54" s="53"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A55" s="68"/>
-      <c r="B55" s="69"/>
-      <c r="C55" s="69"/>
-      <c r="D55" s="69"/>
-      <c r="E55" s="69"/>
-      <c r="F55" s="69"/>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69"/>
-      <c r="I55" s="69"/>
-      <c r="J55" s="69"/>
-      <c r="K55" s="69"/>
-      <c r="L55" s="69"/>
-      <c r="M55" s="69"/>
-      <c r="N55" s="69"/>
-      <c r="O55" s="69"/>
-      <c r="P55" s="69"/>
-      <c r="Q55" s="69"/>
-      <c r="R55" s="69"/>
-      <c r="S55" s="69"/>
-      <c r="T55" s="69"/>
-      <c r="U55" s="69"/>
-      <c r="V55" s="69"/>
-      <c r="W55" s="69"/>
-      <c r="X55" s="69"/>
+      <c r="A55" s="52"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+      <c r="L55" s="53"/>
+      <c r="M55" s="53"/>
+      <c r="N55" s="53"/>
+      <c r="O55" s="53"/>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="53"/>
+      <c r="R55" s="53"/>
+      <c r="S55" s="53"/>
+      <c r="T55" s="53"/>
+      <c r="U55" s="53"/>
+      <c r="V55" s="53"/>
+      <c r="W55" s="53"/>
+      <c r="X55" s="53"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A56" s="68"/>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="69"/>
-      <c r="J56" s="69"/>
-      <c r="K56" s="69"/>
-      <c r="L56" s="69"/>
-      <c r="M56" s="69"/>
-      <c r="N56" s="69"/>
-      <c r="O56" s="69"/>
-      <c r="P56" s="69"/>
-      <c r="Q56" s="69"/>
-      <c r="R56" s="69"/>
-      <c r="S56" s="69"/>
-      <c r="T56" s="69"/>
-      <c r="U56" s="69"/>
-      <c r="V56" s="69"/>
-      <c r="W56" s="69"/>
-      <c r="X56" s="69"/>
+      <c r="A56" s="52"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+      <c r="L56" s="53"/>
+      <c r="M56" s="53"/>
+      <c r="N56" s="53"/>
+      <c r="O56" s="53"/>
+      <c r="P56" s="53"/>
+      <c r="Q56" s="53"/>
+      <c r="R56" s="53"/>
+      <c r="S56" s="53"/>
+      <c r="T56" s="53"/>
+      <c r="U56" s="53"/>
+      <c r="V56" s="53"/>
+      <c r="W56" s="53"/>
+      <c r="X56" s="53"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A57" s="68"/>
-      <c r="B57" s="69"/>
-      <c r="C57" s="69"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69"/>
-      <c r="H57" s="69"/>
-      <c r="I57" s="69"/>
-      <c r="J57" s="69"/>
-      <c r="K57" s="69"/>
-      <c r="L57" s="69"/>
-      <c r="M57" s="69"/>
-      <c r="N57" s="69"/>
-      <c r="O57" s="69"/>
-      <c r="P57" s="69"/>
-      <c r="Q57" s="69"/>
-      <c r="R57" s="69"/>
-      <c r="S57" s="69"/>
-      <c r="T57" s="69"/>
-      <c r="U57" s="69"/>
-      <c r="V57" s="69"/>
-      <c r="W57" s="69"/>
-      <c r="X57" s="69"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="53"/>
+      <c r="K57" s="53"/>
+      <c r="L57" s="53"/>
+      <c r="M57" s="53"/>
+      <c r="N57" s="53"/>
+      <c r="O57" s="53"/>
+      <c r="P57" s="53"/>
+      <c r="Q57" s="53"/>
+      <c r="R57" s="53"/>
+      <c r="S57" s="53"/>
+      <c r="T57" s="53"/>
+      <c r="U57" s="53"/>
+      <c r="V57" s="53"/>
+      <c r="W57" s="53"/>
+      <c r="X57" s="53"/>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A58" s="68"/>
-      <c r="B58" s="69"/>
-      <c r="C58" s="69"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="69"/>
-      <c r="K58" s="69"/>
-      <c r="L58" s="69"/>
-      <c r="M58" s="69"/>
-      <c r="N58" s="69"/>
-      <c r="O58" s="69"/>
-      <c r="P58" s="69"/>
-      <c r="Q58" s="69"/>
-      <c r="R58" s="69"/>
-      <c r="S58" s="69"/>
-      <c r="T58" s="69"/>
-      <c r="U58" s="69"/>
-      <c r="V58" s="69"/>
-      <c r="W58" s="69"/>
-      <c r="X58" s="69"/>
+      <c r="A58" s="52"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="53"/>
+      <c r="L58" s="53"/>
+      <c r="M58" s="53"/>
+      <c r="N58" s="53"/>
+      <c r="O58" s="53"/>
+      <c r="P58" s="53"/>
+      <c r="Q58" s="53"/>
+      <c r="R58" s="53"/>
+      <c r="S58" s="53"/>
+      <c r="T58" s="53"/>
+      <c r="U58" s="53"/>
+      <c r="V58" s="53"/>
+      <c r="W58" s="53"/>
+      <c r="X58" s="53"/>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A59" s="68"/>
-      <c r="B59" s="69"/>
-      <c r="C59" s="69"/>
-      <c r="D59" s="69"/>
-      <c r="E59" s="69"/>
-      <c r="F59" s="69"/>
-      <c r="G59" s="69"/>
-      <c r="H59" s="69"/>
-      <c r="I59" s="69"/>
-      <c r="J59" s="69"/>
-      <c r="K59" s="69"/>
-      <c r="L59" s="69"/>
-      <c r="M59" s="69"/>
-      <c r="N59" s="69"/>
-      <c r="O59" s="69"/>
-      <c r="P59" s="69"/>
-      <c r="Q59" s="69"/>
-      <c r="R59" s="69"/>
-      <c r="S59" s="69"/>
-      <c r="T59" s="69"/>
-      <c r="U59" s="69"/>
-      <c r="V59" s="69"/>
-      <c r="W59" s="69"/>
-      <c r="X59" s="69"/>
+      <c r="A59" s="52"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="53"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="53"/>
+      <c r="L59" s="53"/>
+      <c r="M59" s="53"/>
+      <c r="N59" s="53"/>
+      <c r="O59" s="53"/>
+      <c r="P59" s="53"/>
+      <c r="Q59" s="53"/>
+      <c r="R59" s="53"/>
+      <c r="S59" s="53"/>
+      <c r="T59" s="53"/>
+      <c r="U59" s="53"/>
+      <c r="V59" s="53"/>
+      <c r="W59" s="53"/>
+      <c r="X59" s="53"/>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A60" s="68"/>
-      <c r="B60" s="69"/>
-      <c r="C60" s="69"/>
-      <c r="D60" s="69"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="69"/>
-      <c r="G60" s="69"/>
-      <c r="H60" s="69"/>
-      <c r="I60" s="69"/>
-      <c r="J60" s="69"/>
-      <c r="K60" s="69"/>
-      <c r="L60" s="69"/>
-      <c r="M60" s="69"/>
-      <c r="N60" s="69"/>
-      <c r="O60" s="69"/>
-      <c r="P60" s="69"/>
-      <c r="Q60" s="69"/>
-      <c r="R60" s="69"/>
-      <c r="S60" s="69"/>
-      <c r="T60" s="69"/>
-      <c r="U60" s="69"/>
-      <c r="V60" s="69"/>
-      <c r="W60" s="69"/>
-      <c r="X60" s="69"/>
+      <c r="A60" s="52"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="53"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="53"/>
+      <c r="L60" s="53"/>
+      <c r="M60" s="53"/>
+      <c r="N60" s="53"/>
+      <c r="O60" s="53"/>
+      <c r="P60" s="53"/>
+      <c r="Q60" s="53"/>
+      <c r="R60" s="53"/>
+      <c r="S60" s="53"/>
+      <c r="T60" s="53"/>
+      <c r="U60" s="53"/>
+      <c r="V60" s="53"/>
+      <c r="W60" s="53"/>
+      <c r="X60" s="53"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A61" s="68"/>
-      <c r="B61" s="69"/>
-      <c r="C61" s="69"/>
-      <c r="D61" s="69"/>
-      <c r="E61" s="69"/>
-      <c r="F61" s="69"/>
-      <c r="G61" s="69"/>
-      <c r="H61" s="69"/>
-      <c r="I61" s="69"/>
-      <c r="J61" s="69"/>
-      <c r="K61" s="69"/>
-      <c r="L61" s="69"/>
-      <c r="M61" s="69"/>
-      <c r="N61" s="69"/>
-      <c r="O61" s="69"/>
-      <c r="P61" s="69"/>
-      <c r="Q61" s="69"/>
-      <c r="R61" s="69"/>
-      <c r="S61" s="69"/>
-      <c r="T61" s="69"/>
-      <c r="U61" s="69"/>
-      <c r="V61" s="69"/>
-      <c r="W61" s="69"/>
-      <c r="X61" s="69"/>
+      <c r="A61" s="52"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="53"/>
+      <c r="L61" s="53"/>
+      <c r="M61" s="53"/>
+      <c r="N61" s="53"/>
+      <c r="O61" s="53"/>
+      <c r="P61" s="53"/>
+      <c r="Q61" s="53"/>
+      <c r="R61" s="53"/>
+      <c r="S61" s="53"/>
+      <c r="T61" s="53"/>
+      <c r="U61" s="53"/>
+      <c r="V61" s="53"/>
+      <c r="W61" s="53"/>
+      <c r="X61" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A61:X61"/>
-    <mergeCell ref="A55:X55"/>
-    <mergeCell ref="A56:X56"/>
-    <mergeCell ref="A57:X57"/>
-    <mergeCell ref="A58:X58"/>
-    <mergeCell ref="A59:X59"/>
-    <mergeCell ref="A60:X60"/>
-    <mergeCell ref="A54:X54"/>
-    <mergeCell ref="A43:X43"/>
-    <mergeCell ref="A44:X44"/>
-    <mergeCell ref="A45:X45"/>
-    <mergeCell ref="A46:X46"/>
-    <mergeCell ref="A47:X47"/>
-    <mergeCell ref="A48:X48"/>
-    <mergeCell ref="A49:X49"/>
-    <mergeCell ref="A50:X50"/>
-    <mergeCell ref="A51:X51"/>
-    <mergeCell ref="A52:X52"/>
-    <mergeCell ref="A53:X53"/>
-    <mergeCell ref="A38:X38"/>
-    <mergeCell ref="A39:X39"/>
-    <mergeCell ref="A40:X40"/>
-    <mergeCell ref="A41:X41"/>
-    <mergeCell ref="A17:X17"/>
-    <mergeCell ref="A32:X32"/>
-    <mergeCell ref="A33:X33"/>
-    <mergeCell ref="A34:X34"/>
-    <mergeCell ref="A35:X35"/>
-    <mergeCell ref="A24:X24"/>
-    <mergeCell ref="A25:X25"/>
-    <mergeCell ref="A26:X26"/>
-    <mergeCell ref="A27:X27"/>
-    <mergeCell ref="A28:X28"/>
-    <mergeCell ref="A29:X29"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A2:X2"/>
     <mergeCell ref="A42:X42"/>
     <mergeCell ref="A23:X23"/>
     <mergeCell ref="B18:E18"/>
@@ -4662,16 +4649,40 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="A30:X30"/>
     <mergeCell ref="A31:X31"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A2:X2"/>
+    <mergeCell ref="A38:X38"/>
+    <mergeCell ref="A39:X39"/>
+    <mergeCell ref="A40:X40"/>
+    <mergeCell ref="A41:X41"/>
+    <mergeCell ref="A17:X17"/>
+    <mergeCell ref="A32:X32"/>
+    <mergeCell ref="A33:X33"/>
+    <mergeCell ref="A34:X34"/>
+    <mergeCell ref="A35:X35"/>
+    <mergeCell ref="A24:X24"/>
+    <mergeCell ref="A25:X25"/>
+    <mergeCell ref="A26:X26"/>
+    <mergeCell ref="A27:X27"/>
+    <mergeCell ref="A28:X28"/>
+    <mergeCell ref="A29:X29"/>
+    <mergeCell ref="A54:X54"/>
+    <mergeCell ref="A43:X43"/>
+    <mergeCell ref="A44:X44"/>
+    <mergeCell ref="A45:X45"/>
+    <mergeCell ref="A46:X46"/>
+    <mergeCell ref="A47:X47"/>
+    <mergeCell ref="A48:X48"/>
+    <mergeCell ref="A49:X49"/>
+    <mergeCell ref="A50:X50"/>
+    <mergeCell ref="A51:X51"/>
+    <mergeCell ref="A52:X52"/>
+    <mergeCell ref="A53:X53"/>
+    <mergeCell ref="A61:X61"/>
+    <mergeCell ref="A55:X55"/>
+    <mergeCell ref="A56:X56"/>
+    <mergeCell ref="A57:X57"/>
+    <mergeCell ref="A58:X58"/>
+    <mergeCell ref="A59:X59"/>
+    <mergeCell ref="A60:X60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4699,43 +4710,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="79" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="6"/>
@@ -5080,35 +5091,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87" t="s">
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="86" t="s">
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="86" t="s">
+      <c r="P1" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="86" t="s">
+      <c r="Q1" s="79" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="6"/>
@@ -5124,10 +5135,10 @@
       <c r="AB1" s="6"/>
     </row>
     <row r="2" spans="1:28" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="86"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
@@ -5164,9 +5175,9 @@
       <c r="N2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86" t="s">
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79" t="s">
         <v>4</v>
       </c>
       <c r="R2" s="6"/>

</xml_diff>

<commit_message>
Ver 2.0 Baselined Dec-2018
Ver 2.0 Baseline Dec-2018
</commit_message>
<xml_diff>
--- a/MGMT/PLAN/PP/WORK IN PROGRESS/RAM_MRP.xlsx
+++ b/MGMT/PLAN/PP/WORK IN PROGRESS/RAM_MRP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="178">
   <si>
     <t>Risk Item</t>
   </si>
@@ -575,6 +575,15 @@
   </si>
   <si>
     <t>There could be unknown issues arising while capturing data from actual device/station</t>
+  </si>
+  <si>
+    <t>There may be change from the current Elasticsearch to DynamoDB in the future  (15-Dec-2018)</t>
+  </si>
+  <si>
+    <t>So some of the current codes are written only for current NoSQL db/ElasticSearch. In which case, Those codes have to be written to change to support the new NoSQL db/dynamoDB (15-Dec-2018)</t>
+  </si>
+  <si>
+    <t>Stakeholder engagement, Dec/Jan-2018</t>
   </si>
 </sst>
 </file>
@@ -1278,27 +1287,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1308,6 +1296,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1319,6 +1308,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1337,6 +1328,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1931,7 +1940,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2604,19 +2613,33 @@
       <c r="DF11" s="16"/>
       <c r="DG11" s="16"/>
     </row>
-    <row r="12" spans="1:111" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:111" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50">
         <v>11</v>
       </c>
-      <c r="B12" s="45"/>
+      <c r="B12" s="45" t="s">
+        <v>175</v>
+      </c>
       <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="46"/>
+      <c r="D12" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="J12" s="45"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
@@ -3217,15 +3240,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="19"/>
@@ -3235,42 +3258,42 @@
       <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
     </row>
     <row r="3" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="69"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
@@ -3391,30 +3414,30 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53"/>
-      <c r="T10" s="53"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="53"/>
-      <c r="W10" s="53"/>
-      <c r="X10" s="53"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
     </row>
     <row r="11" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
@@ -3423,13 +3446,13 @@
       <c r="B11" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
     </row>
     <row r="12" spans="1:24" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -3438,13 +3461,13 @@
       <c r="B12" s="40">
         <v>5</v>
       </c>
-      <c r="C12" s="76" t="s">
+      <c r="C12" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
     </row>
     <row r="13" spans="1:24" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
@@ -3453,13 +3476,13 @@
       <c r="B13" s="40">
         <v>4</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="78"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="68"/>
     </row>
     <row r="14" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
@@ -3468,13 +3491,13 @@
       <c r="B14" s="40">
         <v>3</v>
       </c>
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="68"/>
     </row>
     <row r="15" spans="1:24" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
@@ -3483,13 +3506,13 @@
       <c r="B15" s="40">
         <v>2</v>
       </c>
-      <c r="C15" s="76" t="s">
+      <c r="C15" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
     </row>
     <row r="16" spans="1:24" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
@@ -3498,1141 +3521,1165 @@
       <c r="B16" s="41">
         <v>1</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="67"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
     </row>
     <row r="17" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="62"/>
+      <c r="W17" s="62"/>
+      <c r="X17" s="62"/>
     </row>
     <row r="18" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="63" t="s">
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="64"/>
+      <c r="G18" s="78"/>
     </row>
     <row r="19" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="57" t="s">
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="61"/>
+      <c r="G19" s="76"/>
     </row>
     <row r="20" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="57" t="s">
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="61"/>
+      <c r="G20" s="76"/>
     </row>
     <row r="21" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="57" t="s">
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="61"/>
+      <c r="G21" s="76"/>
     </row>
     <row r="22" spans="1:24" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="59" t="s">
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="G22" s="62"/>
+      <c r="G22" s="77"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="53"/>
-      <c r="T23" s="53"/>
-      <c r="U23" s="53"/>
-      <c r="V23" s="53"/>
-      <c r="W23" s="53"/>
-      <c r="X23" s="53"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62"/>
+      <c r="W23" s="62"/>
+      <c r="X23" s="62"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="53"/>
-      <c r="U24" s="53"/>
-      <c r="V24" s="53"/>
-      <c r="W24" s="53"/>
-      <c r="X24" s="53"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="62"/>
+      <c r="R24" s="62"/>
+      <c r="S24" s="62"/>
+      <c r="T24" s="62"/>
+      <c r="U24" s="62"/>
+      <c r="V24" s="62"/>
+      <c r="W24" s="62"/>
+      <c r="X24" s="62"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
-      <c r="P25" s="53"/>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="53"/>
-      <c r="S25" s="53"/>
-      <c r="T25" s="53"/>
-      <c r="U25" s="53"/>
-      <c r="V25" s="53"/>
-      <c r="W25" s="53"/>
-      <c r="X25" s="53"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
+      <c r="S25" s="62"/>
+      <c r="T25" s="62"/>
+      <c r="U25" s="62"/>
+      <c r="V25" s="62"/>
+      <c r="W25" s="62"/>
+      <c r="X25" s="62"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="53"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="53"/>
-      <c r="T26" s="53"/>
-      <c r="U26" s="53"/>
-      <c r="V26" s="53"/>
-      <c r="W26" s="53"/>
-      <c r="X26" s="53"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="62"/>
+      <c r="O26" s="62"/>
+      <c r="P26" s="62"/>
+      <c r="Q26" s="62"/>
+      <c r="R26" s="62"/>
+      <c r="S26" s="62"/>
+      <c r="T26" s="62"/>
+      <c r="U26" s="62"/>
+      <c r="V26" s="62"/>
+      <c r="W26" s="62"/>
+      <c r="X26" s="62"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="53"/>
-      <c r="W27" s="53"/>
-      <c r="X27" s="53"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="62"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="53"/>
-      <c r="S28" s="53"/>
-      <c r="T28" s="53"/>
-      <c r="U28" s="53"/>
-      <c r="V28" s="53"/>
-      <c r="W28" s="53"/>
-      <c r="X28" s="53"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="62"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="62"/>
+      <c r="T28" s="62"/>
+      <c r="U28" s="62"/>
+      <c r="V28" s="62"/>
+      <c r="W28" s="62"/>
+      <c r="X28" s="62"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="53"/>
-      <c r="P29" s="53"/>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="53"/>
-      <c r="T29" s="53"/>
-      <c r="U29" s="53"/>
-      <c r="V29" s="53"/>
-      <c r="W29" s="53"/>
-      <c r="X29" s="53"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
+      <c r="P29" s="62"/>
+      <c r="Q29" s="62"/>
+      <c r="R29" s="62"/>
+      <c r="S29" s="62"/>
+      <c r="T29" s="62"/>
+      <c r="U29" s="62"/>
+      <c r="V29" s="62"/>
+      <c r="W29" s="62"/>
+      <c r="X29" s="62"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="53"/>
-      <c r="O30" s="53"/>
-      <c r="P30" s="53"/>
-      <c r="Q30" s="53"/>
-      <c r="R30" s="53"/>
-      <c r="S30" s="53"/>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
-      <c r="V30" s="53"/>
-      <c r="W30" s="53"/>
-      <c r="X30" s="53"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="62"/>
+      <c r="N30" s="62"/>
+      <c r="O30" s="62"/>
+      <c r="P30" s="62"/>
+      <c r="Q30" s="62"/>
+      <c r="R30" s="62"/>
+      <c r="S30" s="62"/>
+      <c r="T30" s="62"/>
+      <c r="U30" s="62"/>
+      <c r="V30" s="62"/>
+      <c r="W30" s="62"/>
+      <c r="X30" s="62"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="53"/>
-      <c r="P31" s="53"/>
-      <c r="Q31" s="53"/>
-      <c r="R31" s="53"/>
-      <c r="S31" s="53"/>
-      <c r="T31" s="53"/>
-      <c r="U31" s="53"/>
-      <c r="V31" s="53"/>
-      <c r="W31" s="53"/>
-      <c r="X31" s="53"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="62"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="62"/>
+      <c r="S31" s="62"/>
+      <c r="T31" s="62"/>
+      <c r="U31" s="62"/>
+      <c r="V31" s="62"/>
+      <c r="W31" s="62"/>
+      <c r="X31" s="62"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="53"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="53"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="53"/>
-      <c r="R32" s="53"/>
-      <c r="S32" s="53"/>
-      <c r="T32" s="53"/>
-      <c r="U32" s="53"/>
-      <c r="V32" s="53"/>
-      <c r="W32" s="53"/>
-      <c r="X32" s="53"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
+      <c r="P32" s="62"/>
+      <c r="Q32" s="62"/>
+      <c r="R32" s="62"/>
+      <c r="S32" s="62"/>
+      <c r="T32" s="62"/>
+      <c r="U32" s="62"/>
+      <c r="V32" s="62"/>
+      <c r="W32" s="62"/>
+      <c r="X32" s="62"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="53"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="53"/>
-      <c r="S33" s="53"/>
-      <c r="T33" s="53"/>
-      <c r="U33" s="53"/>
-      <c r="V33" s="53"/>
-      <c r="W33" s="53"/>
-      <c r="X33" s="53"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
+      <c r="P33" s="62"/>
+      <c r="Q33" s="62"/>
+      <c r="R33" s="62"/>
+      <c r="S33" s="62"/>
+      <c r="T33" s="62"/>
+      <c r="U33" s="62"/>
+      <c r="V33" s="62"/>
+      <c r="W33" s="62"/>
+      <c r="X33" s="62"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="53"/>
-      <c r="N34" s="53"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="53"/>
-      <c r="S34" s="53"/>
-      <c r="T34" s="53"/>
-      <c r="U34" s="53"/>
-      <c r="V34" s="53"/>
-      <c r="W34" s="53"/>
-      <c r="X34" s="53"/>
+      <c r="A34" s="61"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="62"/>
+      <c r="N34" s="62"/>
+      <c r="O34" s="62"/>
+      <c r="P34" s="62"/>
+      <c r="Q34" s="62"/>
+      <c r="R34" s="62"/>
+      <c r="S34" s="62"/>
+      <c r="T34" s="62"/>
+      <c r="U34" s="62"/>
+      <c r="V34" s="62"/>
+      <c r="W34" s="62"/>
+      <c r="X34" s="62"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="53"/>
-      <c r="S35" s="53"/>
-      <c r="T35" s="53"/>
-      <c r="U35" s="53"/>
-      <c r="V35" s="53"/>
-      <c r="W35" s="53"/>
-      <c r="X35" s="53"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
+      <c r="Q35" s="62"/>
+      <c r="R35" s="62"/>
+      <c r="S35" s="62"/>
+      <c r="T35" s="62"/>
+      <c r="U35" s="62"/>
+      <c r="V35" s="62"/>
+      <c r="W35" s="62"/>
+      <c r="X35" s="62"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="53"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
-      <c r="T36" s="53"/>
-      <c r="U36" s="53"/>
-      <c r="V36" s="53"/>
-      <c r="W36" s="53"/>
-      <c r="X36" s="53"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="62"/>
+      <c r="T36" s="62"/>
+      <c r="U36" s="62"/>
+      <c r="V36" s="62"/>
+      <c r="W36" s="62"/>
+      <c r="X36" s="62"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
-      <c r="O37" s="53"/>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="53"/>
-      <c r="R37" s="53"/>
-      <c r="S37" s="53"/>
-      <c r="T37" s="53"/>
-      <c r="U37" s="53"/>
-      <c r="V37" s="53"/>
-      <c r="W37" s="53"/>
-      <c r="X37" s="53"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="62"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
+      <c r="Q37" s="62"/>
+      <c r="R37" s="62"/>
+      <c r="S37" s="62"/>
+      <c r="T37" s="62"/>
+      <c r="U37" s="62"/>
+      <c r="V37" s="62"/>
+      <c r="W37" s="62"/>
+      <c r="X37" s="62"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
-      <c r="O38" s="53"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="53"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="53"/>
-      <c r="T38" s="53"/>
-      <c r="U38" s="53"/>
-      <c r="V38" s="53"/>
-      <c r="W38" s="53"/>
-      <c r="X38" s="53"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="62"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="62"/>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="62"/>
+      <c r="R38" s="62"/>
+      <c r="S38" s="62"/>
+      <c r="T38" s="62"/>
+      <c r="U38" s="62"/>
+      <c r="V38" s="62"/>
+      <c r="W38" s="62"/>
+      <c r="X38" s="62"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="53"/>
-      <c r="S39" s="53"/>
-      <c r="T39" s="53"/>
-      <c r="U39" s="53"/>
-      <c r="V39" s="53"/>
-      <c r="W39" s="53"/>
-      <c r="X39" s="53"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="62"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="62"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="62"/>
+      <c r="R39" s="62"/>
+      <c r="S39" s="62"/>
+      <c r="T39" s="62"/>
+      <c r="U39" s="62"/>
+      <c r="V39" s="62"/>
+      <c r="W39" s="62"/>
+      <c r="X39" s="62"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A40" s="52"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
-      <c r="O40" s="53"/>
-      <c r="P40" s="53"/>
-      <c r="Q40" s="53"/>
-      <c r="R40" s="53"/>
-      <c r="S40" s="53"/>
-      <c r="T40" s="53"/>
-      <c r="U40" s="53"/>
-      <c r="V40" s="53"/>
-      <c r="W40" s="53"/>
-      <c r="X40" s="53"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62"/>
+      <c r="R40" s="62"/>
+      <c r="S40" s="62"/>
+      <c r="T40" s="62"/>
+      <c r="U40" s="62"/>
+      <c r="V40" s="62"/>
+      <c r="W40" s="62"/>
+      <c r="X40" s="62"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="53"/>
-      <c r="N41" s="53"/>
-      <c r="O41" s="53"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="53"/>
-      <c r="R41" s="53"/>
-      <c r="S41" s="53"/>
-      <c r="T41" s="53"/>
-      <c r="U41" s="53"/>
-      <c r="V41" s="53"/>
-      <c r="W41" s="53"/>
-      <c r="X41" s="53"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="62"/>
+      <c r="M41" s="62"/>
+      <c r="N41" s="62"/>
+      <c r="O41" s="62"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="62"/>
+      <c r="R41" s="62"/>
+      <c r="S41" s="62"/>
+      <c r="T41" s="62"/>
+      <c r="U41" s="62"/>
+      <c r="V41" s="62"/>
+      <c r="W41" s="62"/>
+      <c r="X41" s="62"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="52"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="53"/>
-      <c r="V42" s="53"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="53"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="62"/>
+      <c r="R42" s="62"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
+      <c r="U42" s="62"/>
+      <c r="V42" s="62"/>
+      <c r="W42" s="62"/>
+      <c r="X42" s="62"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A43" s="52"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="53"/>
-      <c r="N43" s="53"/>
-      <c r="O43" s="53"/>
-      <c r="P43" s="53"/>
-      <c r="Q43" s="53"/>
-      <c r="R43" s="53"/>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
-      <c r="U43" s="53"/>
-      <c r="V43" s="53"/>
-      <c r="W43" s="53"/>
-      <c r="X43" s="53"/>
+      <c r="A43" s="61"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
+      <c r="U43" s="62"/>
+      <c r="V43" s="62"/>
+      <c r="W43" s="62"/>
+      <c r="X43" s="62"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A44" s="52"/>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="53"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="53"/>
-      <c r="P44" s="53"/>
-      <c r="Q44" s="53"/>
-      <c r="R44" s="53"/>
-      <c r="S44" s="53"/>
-      <c r="T44" s="53"/>
-      <c r="U44" s="53"/>
-      <c r="V44" s="53"/>
-      <c r="W44" s="53"/>
-      <c r="X44" s="53"/>
+      <c r="A44" s="61"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="62"/>
+      <c r="T44" s="62"/>
+      <c r="U44" s="62"/>
+      <c r="V44" s="62"/>
+      <c r="W44" s="62"/>
+      <c r="X44" s="62"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="53"/>
-      <c r="O45" s="53"/>
-      <c r="P45" s="53"/>
-      <c r="Q45" s="53"/>
-      <c r="R45" s="53"/>
-      <c r="S45" s="53"/>
-      <c r="T45" s="53"/>
-      <c r="U45" s="53"/>
-      <c r="V45" s="53"/>
-      <c r="W45" s="53"/>
-      <c r="X45" s="53"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="62"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="62"/>
+      <c r="R45" s="62"/>
+      <c r="S45" s="62"/>
+      <c r="T45" s="62"/>
+      <c r="U45" s="62"/>
+      <c r="V45" s="62"/>
+      <c r="W45" s="62"/>
+      <c r="X45" s="62"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A46" s="52"/>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="53"/>
-      <c r="L46" s="53"/>
-      <c r="M46" s="53"/>
-      <c r="N46" s="53"/>
-      <c r="O46" s="53"/>
-      <c r="P46" s="53"/>
-      <c r="Q46" s="53"/>
-      <c r="R46" s="53"/>
-      <c r="S46" s="53"/>
-      <c r="T46" s="53"/>
-      <c r="U46" s="53"/>
-      <c r="V46" s="53"/>
-      <c r="W46" s="53"/>
-      <c r="X46" s="53"/>
+      <c r="A46" s="61"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="62"/>
+      <c r="L46" s="62"/>
+      <c r="M46" s="62"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="62"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="62"/>
+      <c r="R46" s="62"/>
+      <c r="S46" s="62"/>
+      <c r="T46" s="62"/>
+      <c r="U46" s="62"/>
+      <c r="V46" s="62"/>
+      <c r="W46" s="62"/>
+      <c r="X46" s="62"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A47" s="52"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="53"/>
-      <c r="L47" s="53"/>
-      <c r="M47" s="53"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="53"/>
-      <c r="P47" s="53"/>
-      <c r="Q47" s="53"/>
-      <c r="R47" s="53"/>
-      <c r="S47" s="53"/>
-      <c r="T47" s="53"/>
-      <c r="U47" s="53"/>
-      <c r="V47" s="53"/>
-      <c r="W47" s="53"/>
-      <c r="X47" s="53"/>
+      <c r="A47" s="61"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="62"/>
+      <c r="L47" s="62"/>
+      <c r="M47" s="62"/>
+      <c r="N47" s="62"/>
+      <c r="O47" s="62"/>
+      <c r="P47" s="62"/>
+      <c r="Q47" s="62"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="62"/>
+      <c r="T47" s="62"/>
+      <c r="U47" s="62"/>
+      <c r="V47" s="62"/>
+      <c r="W47" s="62"/>
+      <c r="X47" s="62"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A48" s="52"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="53"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="53"/>
-      <c r="M48" s="53"/>
-      <c r="N48" s="53"/>
-      <c r="O48" s="53"/>
-      <c r="P48" s="53"/>
-      <c r="Q48" s="53"/>
-      <c r="R48" s="53"/>
-      <c r="S48" s="53"/>
-      <c r="T48" s="53"/>
-      <c r="U48" s="53"/>
-      <c r="V48" s="53"/>
-      <c r="W48" s="53"/>
-      <c r="X48" s="53"/>
+      <c r="A48" s="61"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="62"/>
+      <c r="M48" s="62"/>
+      <c r="N48" s="62"/>
+      <c r="O48" s="62"/>
+      <c r="P48" s="62"/>
+      <c r="Q48" s="62"/>
+      <c r="R48" s="62"/>
+      <c r="S48" s="62"/>
+      <c r="T48" s="62"/>
+      <c r="U48" s="62"/>
+      <c r="V48" s="62"/>
+      <c r="W48" s="62"/>
+      <c r="X48" s="62"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A49" s="52"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="53"/>
-      <c r="J49" s="53"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="53"/>
-      <c r="M49" s="53"/>
-      <c r="N49" s="53"/>
-      <c r="O49" s="53"/>
-      <c r="P49" s="53"/>
-      <c r="Q49" s="53"/>
-      <c r="R49" s="53"/>
-      <c r="S49" s="53"/>
-      <c r="T49" s="53"/>
-      <c r="U49" s="53"/>
-      <c r="V49" s="53"/>
-      <c r="W49" s="53"/>
-      <c r="X49" s="53"/>
+      <c r="A49" s="61"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
+      <c r="K49" s="62"/>
+      <c r="L49" s="62"/>
+      <c r="M49" s="62"/>
+      <c r="N49" s="62"/>
+      <c r="O49" s="62"/>
+      <c r="P49" s="62"/>
+      <c r="Q49" s="62"/>
+      <c r="R49" s="62"/>
+      <c r="S49" s="62"/>
+      <c r="T49" s="62"/>
+      <c r="U49" s="62"/>
+      <c r="V49" s="62"/>
+      <c r="W49" s="62"/>
+      <c r="X49" s="62"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A50" s="52"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="53"/>
-      <c r="M50" s="53"/>
-      <c r="N50" s="53"/>
-      <c r="O50" s="53"/>
-      <c r="P50" s="53"/>
-      <c r="Q50" s="53"/>
-      <c r="R50" s="53"/>
-      <c r="S50" s="53"/>
-      <c r="T50" s="53"/>
-      <c r="U50" s="53"/>
-      <c r="V50" s="53"/>
-      <c r="W50" s="53"/>
-      <c r="X50" s="53"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
+      <c r="L50" s="62"/>
+      <c r="M50" s="62"/>
+      <c r="N50" s="62"/>
+      <c r="O50" s="62"/>
+      <c r="P50" s="62"/>
+      <c r="Q50" s="62"/>
+      <c r="R50" s="62"/>
+      <c r="S50" s="62"/>
+      <c r="T50" s="62"/>
+      <c r="U50" s="62"/>
+      <c r="V50" s="62"/>
+      <c r="W50" s="62"/>
+      <c r="X50" s="62"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A51" s="52"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="53"/>
-      <c r="K51" s="53"/>
-      <c r="L51" s="53"/>
-      <c r="M51" s="53"/>
-      <c r="N51" s="53"/>
-      <c r="O51" s="53"/>
-      <c r="P51" s="53"/>
-      <c r="Q51" s="53"/>
-      <c r="R51" s="53"/>
-      <c r="S51" s="53"/>
-      <c r="T51" s="53"/>
-      <c r="U51" s="53"/>
-      <c r="V51" s="53"/>
-      <c r="W51" s="53"/>
-      <c r="X51" s="53"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="62"/>
+      <c r="J51" s="62"/>
+      <c r="K51" s="62"/>
+      <c r="L51" s="62"/>
+      <c r="M51" s="62"/>
+      <c r="N51" s="62"/>
+      <c r="O51" s="62"/>
+      <c r="P51" s="62"/>
+      <c r="Q51" s="62"/>
+      <c r="R51" s="62"/>
+      <c r="S51" s="62"/>
+      <c r="T51" s="62"/>
+      <c r="U51" s="62"/>
+      <c r="V51" s="62"/>
+      <c r="W51" s="62"/>
+      <c r="X51" s="62"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A52" s="52"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="53"/>
-      <c r="J52" s="53"/>
-      <c r="K52" s="53"/>
-      <c r="L52" s="53"/>
-      <c r="M52" s="53"/>
-      <c r="N52" s="53"/>
-      <c r="O52" s="53"/>
-      <c r="P52" s="53"/>
-      <c r="Q52" s="53"/>
-      <c r="R52" s="53"/>
-      <c r="S52" s="53"/>
-      <c r="T52" s="53"/>
-      <c r="U52" s="53"/>
-      <c r="V52" s="53"/>
-      <c r="W52" s="53"/>
-      <c r="X52" s="53"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="62"/>
+      <c r="L52" s="62"/>
+      <c r="M52" s="62"/>
+      <c r="N52" s="62"/>
+      <c r="O52" s="62"/>
+      <c r="P52" s="62"/>
+      <c r="Q52" s="62"/>
+      <c r="R52" s="62"/>
+      <c r="S52" s="62"/>
+      <c r="T52" s="62"/>
+      <c r="U52" s="62"/>
+      <c r="V52" s="62"/>
+      <c r="W52" s="62"/>
+      <c r="X52" s="62"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A53" s="52"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="53"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="53"/>
-      <c r="L53" s="53"/>
-      <c r="M53" s="53"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53"/>
-      <c r="P53" s="53"/>
-      <c r="Q53" s="53"/>
-      <c r="R53" s="53"/>
-      <c r="S53" s="53"/>
-      <c r="T53" s="53"/>
-      <c r="U53" s="53"/>
-      <c r="V53" s="53"/>
-      <c r="W53" s="53"/>
-      <c r="X53" s="53"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="62"/>
+      <c r="M53" s="62"/>
+      <c r="N53" s="62"/>
+      <c r="O53" s="62"/>
+      <c r="P53" s="62"/>
+      <c r="Q53" s="62"/>
+      <c r="R53" s="62"/>
+      <c r="S53" s="62"/>
+      <c r="T53" s="62"/>
+      <c r="U53" s="62"/>
+      <c r="V53" s="62"/>
+      <c r="W53" s="62"/>
+      <c r="X53" s="62"/>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A54" s="52"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="53"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="53"/>
-      <c r="J54" s="53"/>
-      <c r="K54" s="53"/>
-      <c r="L54" s="53"/>
-      <c r="M54" s="53"/>
-      <c r="N54" s="53"/>
-      <c r="O54" s="53"/>
-      <c r="P54" s="53"/>
-      <c r="Q54" s="53"/>
-      <c r="R54" s="53"/>
-      <c r="S54" s="53"/>
-      <c r="T54" s="53"/>
-      <c r="U54" s="53"/>
-      <c r="V54" s="53"/>
-      <c r="W54" s="53"/>
-      <c r="X54" s="53"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="62"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="62"/>
+      <c r="K54" s="62"/>
+      <c r="L54" s="62"/>
+      <c r="M54" s="62"/>
+      <c r="N54" s="62"/>
+      <c r="O54" s="62"/>
+      <c r="P54" s="62"/>
+      <c r="Q54" s="62"/>
+      <c r="R54" s="62"/>
+      <c r="S54" s="62"/>
+      <c r="T54" s="62"/>
+      <c r="U54" s="62"/>
+      <c r="V54" s="62"/>
+      <c r="W54" s="62"/>
+      <c r="X54" s="62"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A55" s="52"/>
-      <c r="B55" s="53"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="53"/>
-      <c r="H55" s="53"/>
-      <c r="I55" s="53"/>
-      <c r="J55" s="53"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="53"/>
-      <c r="M55" s="53"/>
-      <c r="N55" s="53"/>
-      <c r="O55" s="53"/>
-      <c r="P55" s="53"/>
-      <c r="Q55" s="53"/>
-      <c r="R55" s="53"/>
-      <c r="S55" s="53"/>
-      <c r="T55" s="53"/>
-      <c r="U55" s="53"/>
-      <c r="V55" s="53"/>
-      <c r="W55" s="53"/>
-      <c r="X55" s="53"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="62"/>
+      <c r="F55" s="62"/>
+      <c r="G55" s="62"/>
+      <c r="H55" s="62"/>
+      <c r="I55" s="62"/>
+      <c r="J55" s="62"/>
+      <c r="K55" s="62"/>
+      <c r="L55" s="62"/>
+      <c r="M55" s="62"/>
+      <c r="N55" s="62"/>
+      <c r="O55" s="62"/>
+      <c r="P55" s="62"/>
+      <c r="Q55" s="62"/>
+      <c r="R55" s="62"/>
+      <c r="S55" s="62"/>
+      <c r="T55" s="62"/>
+      <c r="U55" s="62"/>
+      <c r="V55" s="62"/>
+      <c r="W55" s="62"/>
+      <c r="X55" s="62"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="53"/>
-      <c r="I56" s="53"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="53"/>
-      <c r="M56" s="53"/>
-      <c r="N56" s="53"/>
-      <c r="O56" s="53"/>
-      <c r="P56" s="53"/>
-      <c r="Q56" s="53"/>
-      <c r="R56" s="53"/>
-      <c r="S56" s="53"/>
-      <c r="T56" s="53"/>
-      <c r="U56" s="53"/>
-      <c r="V56" s="53"/>
-      <c r="W56" s="53"/>
-      <c r="X56" s="53"/>
+      <c r="A56" s="61"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="62"/>
+      <c r="H56" s="62"/>
+      <c r="I56" s="62"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="62"/>
+      <c r="L56" s="62"/>
+      <c r="M56" s="62"/>
+      <c r="N56" s="62"/>
+      <c r="O56" s="62"/>
+      <c r="P56" s="62"/>
+      <c r="Q56" s="62"/>
+      <c r="R56" s="62"/>
+      <c r="S56" s="62"/>
+      <c r="T56" s="62"/>
+      <c r="U56" s="62"/>
+      <c r="V56" s="62"/>
+      <c r="W56" s="62"/>
+      <c r="X56" s="62"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A57" s="52"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="53"/>
-      <c r="H57" s="53"/>
-      <c r="I57" s="53"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="53"/>
-      <c r="L57" s="53"/>
-      <c r="M57" s="53"/>
-      <c r="N57" s="53"/>
-      <c r="O57" s="53"/>
-      <c r="P57" s="53"/>
-      <c r="Q57" s="53"/>
-      <c r="R57" s="53"/>
-      <c r="S57" s="53"/>
-      <c r="T57" s="53"/>
-      <c r="U57" s="53"/>
-      <c r="V57" s="53"/>
-      <c r="W57" s="53"/>
-      <c r="X57" s="53"/>
+      <c r="A57" s="61"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="62"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="62"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="62"/>
+      <c r="L57" s="62"/>
+      <c r="M57" s="62"/>
+      <c r="N57" s="62"/>
+      <c r="O57" s="62"/>
+      <c r="P57" s="62"/>
+      <c r="Q57" s="62"/>
+      <c r="R57" s="62"/>
+      <c r="S57" s="62"/>
+      <c r="T57" s="62"/>
+      <c r="U57" s="62"/>
+      <c r="V57" s="62"/>
+      <c r="W57" s="62"/>
+      <c r="X57" s="62"/>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A58" s="52"/>
-      <c r="B58" s="53"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="53"/>
-      <c r="M58" s="53"/>
-      <c r="N58" s="53"/>
-      <c r="O58" s="53"/>
-      <c r="P58" s="53"/>
-      <c r="Q58" s="53"/>
-      <c r="R58" s="53"/>
-      <c r="S58" s="53"/>
-      <c r="T58" s="53"/>
-      <c r="U58" s="53"/>
-      <c r="V58" s="53"/>
-      <c r="W58" s="53"/>
-      <c r="X58" s="53"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="62"/>
+      <c r="H58" s="62"/>
+      <c r="I58" s="62"/>
+      <c r="J58" s="62"/>
+      <c r="K58" s="62"/>
+      <c r="L58" s="62"/>
+      <c r="M58" s="62"/>
+      <c r="N58" s="62"/>
+      <c r="O58" s="62"/>
+      <c r="P58" s="62"/>
+      <c r="Q58" s="62"/>
+      <c r="R58" s="62"/>
+      <c r="S58" s="62"/>
+      <c r="T58" s="62"/>
+      <c r="U58" s="62"/>
+      <c r="V58" s="62"/>
+      <c r="W58" s="62"/>
+      <c r="X58" s="62"/>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A59" s="52"/>
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="53"/>
-      <c r="H59" s="53"/>
-      <c r="I59" s="53"/>
-      <c r="J59" s="53"/>
-      <c r="K59" s="53"/>
-      <c r="L59" s="53"/>
-      <c r="M59" s="53"/>
-      <c r="N59" s="53"/>
-      <c r="O59" s="53"/>
-      <c r="P59" s="53"/>
-      <c r="Q59" s="53"/>
-      <c r="R59" s="53"/>
-      <c r="S59" s="53"/>
-      <c r="T59" s="53"/>
-      <c r="U59" s="53"/>
-      <c r="V59" s="53"/>
-      <c r="W59" s="53"/>
-      <c r="X59" s="53"/>
+      <c r="A59" s="61"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="62"/>
+      <c r="K59" s="62"/>
+      <c r="L59" s="62"/>
+      <c r="M59" s="62"/>
+      <c r="N59" s="62"/>
+      <c r="O59" s="62"/>
+      <c r="P59" s="62"/>
+      <c r="Q59" s="62"/>
+      <c r="R59" s="62"/>
+      <c r="S59" s="62"/>
+      <c r="T59" s="62"/>
+      <c r="U59" s="62"/>
+      <c r="V59" s="62"/>
+      <c r="W59" s="62"/>
+      <c r="X59" s="62"/>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A60" s="52"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="53"/>
-      <c r="G60" s="53"/>
-      <c r="H60" s="53"/>
-      <c r="I60" s="53"/>
-      <c r="J60" s="53"/>
-      <c r="K60" s="53"/>
-      <c r="L60" s="53"/>
-      <c r="M60" s="53"/>
-      <c r="N60" s="53"/>
-      <c r="O60" s="53"/>
-      <c r="P60" s="53"/>
-      <c r="Q60" s="53"/>
-      <c r="R60" s="53"/>
-      <c r="S60" s="53"/>
-      <c r="T60" s="53"/>
-      <c r="U60" s="53"/>
-      <c r="V60" s="53"/>
-      <c r="W60" s="53"/>
-      <c r="X60" s="53"/>
+      <c r="A60" s="61"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="62"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="62"/>
+      <c r="J60" s="62"/>
+      <c r="K60" s="62"/>
+      <c r="L60" s="62"/>
+      <c r="M60" s="62"/>
+      <c r="N60" s="62"/>
+      <c r="O60" s="62"/>
+      <c r="P60" s="62"/>
+      <c r="Q60" s="62"/>
+      <c r="R60" s="62"/>
+      <c r="S60" s="62"/>
+      <c r="T60" s="62"/>
+      <c r="U60" s="62"/>
+      <c r="V60" s="62"/>
+      <c r="W60" s="62"/>
+      <c r="X60" s="62"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A61" s="52"/>
-      <c r="B61" s="53"/>
-      <c r="C61" s="53"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="53"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="53"/>
-      <c r="L61" s="53"/>
-      <c r="M61" s="53"/>
-      <c r="N61" s="53"/>
-      <c r="O61" s="53"/>
-      <c r="P61" s="53"/>
-      <c r="Q61" s="53"/>
-      <c r="R61" s="53"/>
-      <c r="S61" s="53"/>
-      <c r="T61" s="53"/>
-      <c r="U61" s="53"/>
-      <c r="V61" s="53"/>
-      <c r="W61" s="53"/>
-      <c r="X61" s="53"/>
+      <c r="A61" s="61"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
+      <c r="I61" s="62"/>
+      <c r="J61" s="62"/>
+      <c r="K61" s="62"/>
+      <c r="L61" s="62"/>
+      <c r="M61" s="62"/>
+      <c r="N61" s="62"/>
+      <c r="O61" s="62"/>
+      <c r="P61" s="62"/>
+      <c r="Q61" s="62"/>
+      <c r="R61" s="62"/>
+      <c r="S61" s="62"/>
+      <c r="T61" s="62"/>
+      <c r="U61" s="62"/>
+      <c r="V61" s="62"/>
+      <c r="W61" s="62"/>
+      <c r="X61" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A10:X10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A2:X2"/>
+    <mergeCell ref="A61:X61"/>
+    <mergeCell ref="A55:X55"/>
+    <mergeCell ref="A56:X56"/>
+    <mergeCell ref="A57:X57"/>
+    <mergeCell ref="A58:X58"/>
+    <mergeCell ref="A59:X59"/>
+    <mergeCell ref="A60:X60"/>
+    <mergeCell ref="A54:X54"/>
+    <mergeCell ref="A43:X43"/>
+    <mergeCell ref="A44:X44"/>
+    <mergeCell ref="A45:X45"/>
+    <mergeCell ref="A46:X46"/>
+    <mergeCell ref="A47:X47"/>
+    <mergeCell ref="A48:X48"/>
+    <mergeCell ref="A49:X49"/>
+    <mergeCell ref="A50:X50"/>
+    <mergeCell ref="A51:X51"/>
+    <mergeCell ref="A52:X52"/>
+    <mergeCell ref="A53:X53"/>
+    <mergeCell ref="A38:X38"/>
+    <mergeCell ref="A39:X39"/>
+    <mergeCell ref="A40:X40"/>
+    <mergeCell ref="A41:X41"/>
+    <mergeCell ref="A17:X17"/>
+    <mergeCell ref="A32:X32"/>
+    <mergeCell ref="A33:X33"/>
+    <mergeCell ref="A34:X34"/>
+    <mergeCell ref="A35:X35"/>
+    <mergeCell ref="A24:X24"/>
+    <mergeCell ref="A25:X25"/>
+    <mergeCell ref="A26:X26"/>
+    <mergeCell ref="A27:X27"/>
+    <mergeCell ref="A28:X28"/>
+    <mergeCell ref="A29:X29"/>
     <mergeCell ref="A42:X42"/>
     <mergeCell ref="A23:X23"/>
     <mergeCell ref="B18:E18"/>
@@ -4649,40 +4696,16 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="A30:X30"/>
     <mergeCell ref="A31:X31"/>
-    <mergeCell ref="A38:X38"/>
-    <mergeCell ref="A39:X39"/>
-    <mergeCell ref="A40:X40"/>
-    <mergeCell ref="A41:X41"/>
-    <mergeCell ref="A17:X17"/>
-    <mergeCell ref="A32:X32"/>
-    <mergeCell ref="A33:X33"/>
-    <mergeCell ref="A34:X34"/>
-    <mergeCell ref="A35:X35"/>
-    <mergeCell ref="A24:X24"/>
-    <mergeCell ref="A25:X25"/>
-    <mergeCell ref="A26:X26"/>
-    <mergeCell ref="A27:X27"/>
-    <mergeCell ref="A28:X28"/>
-    <mergeCell ref="A29:X29"/>
-    <mergeCell ref="A54:X54"/>
-    <mergeCell ref="A43:X43"/>
-    <mergeCell ref="A44:X44"/>
-    <mergeCell ref="A45:X45"/>
-    <mergeCell ref="A46:X46"/>
-    <mergeCell ref="A47:X47"/>
-    <mergeCell ref="A48:X48"/>
-    <mergeCell ref="A49:X49"/>
-    <mergeCell ref="A50:X50"/>
-    <mergeCell ref="A51:X51"/>
-    <mergeCell ref="A52:X52"/>
-    <mergeCell ref="A53:X53"/>
-    <mergeCell ref="A61:X61"/>
-    <mergeCell ref="A55:X55"/>
-    <mergeCell ref="A56:X56"/>
-    <mergeCell ref="A57:X57"/>
-    <mergeCell ref="A58:X58"/>
-    <mergeCell ref="A59:X59"/>
-    <mergeCell ref="A60:X60"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:X10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>